<commit_message>
Update csv: added more authors, books and quantity set to 20k
</commit_message>
<xml_diff>
--- a/csv/sources/author.xlsx
+++ b/csv/sources/author.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Casa\Desktop\hyp-project\csv\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Casa\Desktop\hyp-project\csv\sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3648882D-EC03-499A-9185-2AC38BAC1131}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D774638-1691-4345-A7EE-AFC980271401}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{55366492-BCD1-4018-9CE8-CD446D6216F5}"/>
+    <workbookView xWindow="13710" yWindow="4180" windowWidth="10800" windowHeight="7360" xr2:uid="{55366492-BCD1-4018-9CE8-CD446D6216F5}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="97">
   <si>
     <t>author_id</t>
   </si>
@@ -161,12 +161,6 @@
     <t>Gillian Flynn</t>
   </si>
   <si>
-    <t>Michelle Obama</t>
-  </si>
-  <si>
-    <t>Michelle Obama is an American lawyer, university administrator and writer, who was First Lady of the United States from 2009 to 2017. She is married to the 44th U.S. President, Barack Obama, and was the first African-American First Lady.</t>
-  </si>
-  <si>
     <t>Donald Arthur Norman (born December 25, 1935) is a researcher, professor, and author. Norman is the director of The Design Lab at University of California, San Diego. He is best known for his books on design, especially The Design of Everyday Things. He is widely regarded for his expertise in the fields of design, usability engineering, and cognitive science. He is a co-founder and consultant with the Nielsen Norman Group. </t>
   </si>
   <si>
@@ -230,20 +224,116 @@
     <t>gillian_flynn.jpeg</t>
   </si>
   <si>
-    <t>michelle_obama.jpeg</t>
-  </si>
-  <si>
     <t>giorgia_lupi.jpeg</t>
   </si>
   <si>
     <t>ingrid_fetell_lee.jpeg</t>
+  </si>
+  <si>
+    <t>Sir Terence David John Pratchett OBE was an English author of fantasy novels, especially comical works. He is best known for his Discworld series of 41 novels. Pratchett's first novel, The Carpet People, was published in 1971.</t>
+  </si>
+  <si>
+    <t>Terry Pratchett</t>
+  </si>
+  <si>
+    <t>Stefanie Posavec is a London-based information designer whose work focuses on non-traditional representations of data, born in 1981. She co-authored the 2016 book Dear Data with Giorgia Lupi.</t>
+  </si>
+  <si>
+    <t>Stefanie Posavec</t>
+  </si>
+  <si>
+    <t>Robin Wasserman is an American young adult novelist. Wasserman grew up outside of Philadelphia and graduated from Harvard University and UCLA. Before she was an author she was an associate editor at a children's book publisher. She is currently living in Brooklyn, New York.</t>
+  </si>
+  <si>
+    <t>Robin Wasserman</t>
+  </si>
+  <si>
+    <t>Maureen Johnson is an American author of young adult fiction. She has published thirteen young adult novels to date, including such series as the Truly Devious novels, the Shades of London series, and Suite Scarlett. Johnson's work has also appeared in numerous written anthologies, and comprises notable collaborative works with her contemporaries.</t>
+  </si>
+  <si>
+    <t>Maureen Johnson</t>
+  </si>
+  <si>
+    <t>Sarah Rees Brennan is the author of the Demon’s Lexicon trilogy and the co-author, with Justine Larbalestier, of Team Human, and the Lynburn Legacy series which begins with Unspoken, a romantic Gothic mystery about a girl named Kami Glass, who discovers her imaginary friend is a real boy.</t>
+  </si>
+  <si>
+    <t>Sarah Rees Brennan</t>
+  </si>
+  <si>
+    <t>Judith Lewis, better known by her pen name Cassandra Clare, is an American author of young adult fiction, best known for her bestselling series The Mortal Instruments. In 2004, Clare started working on her first-published novel, City of Bones, inspired by the urban landscape of Manhattan, and released by Simon &amp; Schuster in 2007.</t>
+  </si>
+  <si>
+    <t>Cassandra Clare</t>
+  </si>
+  <si>
+    <t>Adam Silvera</t>
+  </si>
+  <si>
+    <t>Rebecca "Becky" Albertalli is an American author of young adult fiction, best known for Simon vs. the Homo Sapiens Agenda, which was adapted into the 2018 movie Love, Simon. A sequel to Simon vs. the Homo Sapiens Agenda, titled Leah on the Offbeat was released in 2018 and won the Goodreads Choice Award for Best Young Adult Fiction.</t>
+  </si>
+  <si>
+    <t>Becky Albertalli</t>
+  </si>
+  <si>
+    <t>Lauren Willig is a New York Times bestselling author of historical novels. She is best known for her "Pink Carnation" series, which follows a collection of Napoleonic-Era British spies, similar to the Scarlet Pimpernel, as they fight for Britain and fall in love.</t>
+  </si>
+  <si>
+    <t>Lauren Willig</t>
+  </si>
+  <si>
+    <t>Beatriz Williams is the New York Times, USA Today, and internationally bestselling author of The Summer Wives, The Secret Life of Violet Grant, A Hundred Summers, A Certain Age, and several other works of historical fiction.</t>
+  </si>
+  <si>
+    <t>Beatriz Williams</t>
+  </si>
+  <si>
+    <t>Karen White is a New York Times bestselling American author of more than twenty-five novels. On Folly Beach, published in May 2010, was a NYT bestseller. Most of White's novels are based in the low-country of the southeastern United States. White currently has 26 novels published with the latest book, Dreams of Falling in June 2018.</t>
+  </si>
+  <si>
+    <t>Karen White</t>
+  </si>
+  <si>
+    <t>karen_white.jpeg</t>
+  </si>
+  <si>
+    <t>beatriz_williams.jpeg</t>
+  </si>
+  <si>
+    <t>lauren_willig.jpeg</t>
+  </si>
+  <si>
+    <t>becky_albertalli.jpeg</t>
+  </si>
+  <si>
+    <t>adam_silvera.jpeg</t>
+  </si>
+  <si>
+    <t>cassandra_clare.jpeg</t>
+  </si>
+  <si>
+    <t>sarah_brennan.jpeg</t>
+  </si>
+  <si>
+    <t>maureen_johnson.jpeg</t>
+  </si>
+  <si>
+    <t>robin_wasserman.jpeg</t>
+  </si>
+  <si>
+    <t>stefanie_posavec.jpeg</t>
+  </si>
+  <si>
+    <t>terry_pratchett.jpeg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adam Silvera is a New York Times Bestselling author of young adult fiction, best known for his novels They Both Die at the End, What If It's Us, and More Happy Than Not. Silvera started writing when he was around 10 or 11, initially working on fan fiction. Silvera has worked as a barista, bookseller, and reviewer for Shelf Awareness before becoming a published writer. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -268,8 +358,31 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Asap"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF1D252C"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -279,6 +392,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE1F1ED"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -310,7 +429,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -326,6 +445,24 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -641,10 +778,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25D6DAC7-F16B-4C4F-BA6A-3EE9DFB1974B}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27:A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -680,7 +817,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="51.5" thickBot="1">
@@ -691,10 +828,10 @@
         <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="51.5" thickBot="1">
@@ -705,10 +842,10 @@
         <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="39" thickBot="1">
@@ -722,7 +859,7 @@
         <v>9</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="51.5" thickBot="1">
@@ -736,7 +873,7 @@
         <v>11</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="51.5" thickBot="1">
@@ -750,7 +887,7 @@
         <v>13</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="26.5" thickBot="1">
@@ -764,7 +901,7 @@
         <v>15</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="39" thickBot="1">
@@ -778,7 +915,7 @@
         <v>17</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="64" thickBot="1">
@@ -792,7 +929,7 @@
         <v>19</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15" thickBot="1">
@@ -806,7 +943,7 @@
         <v>21</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="39" thickBot="1">
@@ -820,7 +957,7 @@
         <v>23</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="64" thickBot="1">
@@ -834,7 +971,7 @@
         <v>25</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="89" thickBot="1">
@@ -848,7 +985,7 @@
         <v>27</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="51.5" thickBot="1">
@@ -862,7 +999,7 @@
         <v>29</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="51.5" thickBot="1">
@@ -876,7 +1013,7 @@
         <v>31</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="36" thickBot="1">
@@ -890,7 +1027,7 @@
         <v>33</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="47.5" thickBot="1">
@@ -904,7 +1041,7 @@
         <v>35</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="24.5" thickBot="1">
@@ -918,7 +1055,7 @@
         <v>37</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="36" thickBot="1">
@@ -932,7 +1069,7 @@
         <v>39</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="39" thickBot="1">
@@ -943,24 +1080,164 @@
         <v>40</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="26.5" thickBot="1">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="38" thickBot="1">
       <c r="A22">
         <v>10000020</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>42</v>
+      <c r="B22" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="D22" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="23.5" thickBot="1">
+      <c r="A23">
+        <v>10000021</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="23.5" thickBot="1">
+      <c r="A24">
+        <v>10000022</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="35" thickBot="1">
+      <c r="A25">
+        <v>10000023</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="38" thickBot="1">
+      <c r="A26">
+        <v>10000024</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="38" thickBot="1">
+      <c r="A27">
+        <v>10000025</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="38" thickBot="1">
+      <c r="A28">
+        <v>10000026</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="38" thickBot="1">
+      <c r="A29">
+        <v>10000027</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="38" thickBot="1">
+      <c r="A30">
+        <v>10000028</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="25.5" thickBot="1">
+      <c r="A31">
+        <v>10000029</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="25.5" thickBot="1">
+      <c r="A32">
+        <v>10000030</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C32" s="8" t="s">
         <v>64</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>